<commit_message>
Updated LoadExcelData and added TimeSeries script
</commit_message>
<xml_diff>
--- a/traffic_data.xlsx
+++ b/traffic_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhnamnguyen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhnamnguyen/Desktop/TrafficLight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B610EC9-CC56-1D4C-B8F7-F48E619F2002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA18C2-A19D-4144-AE6E-7CC2AA0436B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17240" xr2:uid="{BAB280F7-8F99-4347-B136-DE927E1DC0F7}"/>
   </bookViews>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8945BEEB-E5C1-CD4A-ABA7-70D9A64B9A68}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,6 +500,104 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>